<commit_message>
updated Facebook and Twitter data
</commit_message>
<xml_diff>
--- a/data/analysis/social_media_analytics/museums_on_fb_temporal-all_mus-M.xlsx
+++ b/data/analysis/social_media_analytics/museums_on_fb_temporal-all_mus-M.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="4">
   <si>
     <t>ts</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,7 +409,7 @@
         <v>43496</v>
       </c>
       <c r="B2">
-        <v>1124</v>
+        <v>1771</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -420,7 +420,7 @@
         <v>43524</v>
       </c>
       <c r="B3">
-        <v>1134</v>
+        <v>1792</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -431,7 +431,7 @@
         <v>43555</v>
       </c>
       <c r="B4">
-        <v>1149</v>
+        <v>1830</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -442,7 +442,7 @@
         <v>43585</v>
       </c>
       <c r="B5">
-        <v>1152</v>
+        <v>1840</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -453,7 +453,7 @@
         <v>43616</v>
       </c>
       <c r="B6">
-        <v>1155</v>
+        <v>1847</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -464,7 +464,7 @@
         <v>43646</v>
       </c>
       <c r="B7">
-        <v>1160</v>
+        <v>1843</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -475,7 +475,7 @@
         <v>43677</v>
       </c>
       <c r="B8">
-        <v>1159</v>
+        <v>1837</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -486,7 +486,7 @@
         <v>43708</v>
       </c>
       <c r="B9">
-        <v>1162</v>
+        <v>1838</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -497,7 +497,7 @@
         <v>43738</v>
       </c>
       <c r="B10">
-        <v>1164</v>
+        <v>1839</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -508,7 +508,7 @@
         <v>43769</v>
       </c>
       <c r="B11">
-        <v>1165</v>
+        <v>1850</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -519,7 +519,7 @@
         <v>43799</v>
       </c>
       <c r="B12">
-        <v>1156</v>
+        <v>1815</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -530,7 +530,7 @@
         <v>43830</v>
       </c>
       <c r="B13">
-        <v>1144</v>
+        <v>1784</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -541,7 +541,7 @@
         <v>43861</v>
       </c>
       <c r="B14">
-        <v>1136</v>
+        <v>1786</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -552,7 +552,7 @@
         <v>43890</v>
       </c>
       <c r="B15">
-        <v>1159</v>
+        <v>1817</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -563,7 +563,7 @@
         <v>43921</v>
       </c>
       <c r="B16">
-        <v>1181</v>
+        <v>1893</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -574,7 +574,7 @@
         <v>43951</v>
       </c>
       <c r="B17">
-        <v>1120</v>
+        <v>1739</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -585,7 +585,7 @@
         <v>43982</v>
       </c>
       <c r="B18">
-        <v>1079</v>
+        <v>1676</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -596,7 +596,7 @@
         <v>44012</v>
       </c>
       <c r="B19">
-        <v>1105</v>
+        <v>1707</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -607,7 +607,7 @@
         <v>44043</v>
       </c>
       <c r="B20">
-        <v>1113</v>
+        <v>1742</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -618,7 +618,7 @@
         <v>44074</v>
       </c>
       <c r="B21">
-        <v>1113</v>
+        <v>1726</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -629,7 +629,7 @@
         <v>44104</v>
       </c>
       <c r="B22">
-        <v>1118</v>
+        <v>1727</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -640,7 +640,7 @@
         <v>44135</v>
       </c>
       <c r="B23">
-        <v>1124</v>
+        <v>1739</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -651,7 +651,7 @@
         <v>44165</v>
       </c>
       <c r="B24">
-        <v>1133</v>
+        <v>1751</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -662,7 +662,7 @@
         <v>44196</v>
       </c>
       <c r="B25">
-        <v>1129</v>
+        <v>1736</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -673,7 +673,7 @@
         <v>44227</v>
       </c>
       <c r="B26">
-        <v>1095</v>
+        <v>1643</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -684,7 +684,7 @@
         <v>44255</v>
       </c>
       <c r="B27">
-        <v>1079</v>
+        <v>1657</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -695,7 +695,7 @@
         <v>44286</v>
       </c>
       <c r="B28">
-        <v>1119</v>
+        <v>1714</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -706,7 +706,7 @@
         <v>44316</v>
       </c>
       <c r="B29">
-        <v>1119</v>
+        <v>1760</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -717,7 +717,7 @@
         <v>44347</v>
       </c>
       <c r="B30">
-        <v>1154</v>
+        <v>1824</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -728,7 +728,7 @@
         <v>44377</v>
       </c>
       <c r="B31">
-        <v>1143</v>
+        <v>1823</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -739,7 +739,7 @@
         <v>44408</v>
       </c>
       <c r="B32">
-        <v>1145</v>
+        <v>1822</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -750,7 +750,7 @@
         <v>44439</v>
       </c>
       <c r="B33">
-        <v>1141</v>
+        <v>1816</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -761,9 +761,97 @@
         <v>44469</v>
       </c>
       <c r="B34">
-        <v>1148</v>
+        <v>1838</v>
       </c>
       <c r="C34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2">
+        <v>44500</v>
+      </c>
+      <c r="B35">
+        <v>1824</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2">
+        <v>44530</v>
+      </c>
+      <c r="B36">
+        <v>1821</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2">
+        <v>44561</v>
+      </c>
+      <c r="B37">
+        <v>1783</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2">
+        <v>44592</v>
+      </c>
+      <c r="B38">
+        <v>1730</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2">
+        <v>44620</v>
+      </c>
+      <c r="B39">
+        <v>1832</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2">
+        <v>44651</v>
+      </c>
+      <c r="B40">
+        <v>1875</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2">
+        <v>44681</v>
+      </c>
+      <c r="B41">
+        <v>1913</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
+        <v>44712</v>
+      </c>
+      <c r="B42">
+        <v>1940</v>
+      </c>
+      <c r="C42" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>